<commit_message>
20211230 CRE20-023-68	COVID19 – Phase 68         Add child document for COVID19 Scheme         Allow input Chinese Name for child document         Add 2nd dose warning message for 12-17yo         Enhance CCCode Mapping         Obsolete HA_MingLiu
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/PPC0001-Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/PPC0001-Template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swl109\Documents\GitHub\EHS\EHS2019\EHS\ExcelGenerator\Template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="6075" windowWidth="19260" windowHeight="6000" tabRatio="679"/>
   </bookViews>
@@ -130,13 +135,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0_ "/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -211,7 +216,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -225,16 +230,10 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="HA_MingLiu"/>
-      <family val="3"/>
-      <charset val="136"/>
     </font>
   </fonts>
   <fills count="2">
@@ -278,7 +277,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -292,7 +291,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -339,9 +338,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -371,6 +367,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -419,7 +418,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -454,7 +453,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -667,13 +666,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="12" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -681,7 +680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>25</v>
       </c>
@@ -689,10 +688,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
     </row>
-    <row r="4" spans="1:2" ht="15.75">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -710,22 +709,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.7109375" style="12" customWidth="1"/>
     <col min="2" max="2" width="52.7109375" style="19" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="20"/>
     </row>
@@ -742,41 +741,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="9" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="21" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="10" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" style="10" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" style="21" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" style="10" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" style="10" customWidth="1"/>
-    <col min="10" max="10" width="36.7109375" style="21" customWidth="1"/>
-    <col min="11" max="11" width="50.7109375" style="10" customWidth="1"/>
-    <col min="12" max="12" width="50.7109375" style="21" customWidth="1"/>
+    <col min="9" max="10" width="36.7109375" style="10" customWidth="1"/>
+    <col min="11" max="12" width="50.7109375" style="10" customWidth="1"/>
     <col min="13" max="13" width="20.85546875" style="10" customWidth="1"/>
     <col min="14" max="17" width="20.7109375" style="10" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:17" ht="15">
-      <c r="D2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="L2" s="10"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75">
+    </row>
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>28</v>
       </c>
@@ -843,114 +830,114 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" style="10" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="16"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="16"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="16"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="16"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="16"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="16"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="16"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="16"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="16"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
     </row>
   </sheetData>
@@ -966,36 +953,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="23" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.85546875" style="23" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="1" width="9" style="22" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" customHeight="1"/>
-    <row r="3" spans="1:4" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A3" s="24" t="s">
+    <row r="2" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" s="24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1009,13 +996,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>

</xml_diff>